<commit_message>
Small preparations for vk parser ading
</commit_message>
<xml_diff>
--- a/data/temp_sources.xlsx
+++ b/data/temp_sources.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,14 +479,18 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://vk.com/ff_mgu</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>https://t.me/physics_msu_official</t>
         </is>
       </c>
       <c r="G2" s="1" t="n">
-        <v>46068.63083333334</v>
+        <v>46070</v>
       </c>
     </row>
     <row r="3">
@@ -513,7 +517,34 @@
         </is>
       </c>
       <c r="G3" s="1" t="n">
-        <v>45910.66563657407</v>
+        <v>45910</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Оптики, спектроскопии и физики наносистем</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Экспериментальной и теоретической физики</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>А</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>http://vk.com/club215377281</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" s="1" t="n">
+        <v>46056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>